<commit_message>
CAMBIOS GORDOS PREPRAR PARA XAI
</commit_message>
<xml_diff>
--- a/articulo 1 XAI/Articulos_dosFases.xlsx
+++ b/articulo 1 XAI/Articulos_dosFases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miumh-my.sharepoint.com/personal/ricardo_gonzalezm_miumh_umh_es/Documents/Documentos/Cafee/articulo 1 XAI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D63E4930-6956-4C32-AC3A-A5221AF6B2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{D63E4930-6956-4C32-AC3A-A5221AF6B2B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3141198-D27B-4D2E-A045-7A9552943F35}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{546FD665-A4C1-4419-A88D-885BF4821FCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Num</t>
   </si>
@@ -57,6 +57,48 @@
   </si>
   <si>
     <t>A combined machine learning algorithms and DEA method for measuring and predicting the efficiency of Chinese manufacturing listed companies</t>
+  </si>
+  <si>
+    <t>https://www.jsoftware.us/vol8/jsw0801-04.pdf</t>
+  </si>
+  <si>
+    <t>Supplier’s Efficiency and Performance  Evaluation using DEA-SVM Approach</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0360835208001113</t>
+  </si>
+  <si>
+    <t>A combined neural network and DEA for measuring efficiency of large scale datasets</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0959652620321533#fig2</t>
+  </si>
+  <si>
+    <t>Farm efficiency estimation using a hybrid approach of machine-learning and data envelopment analysis: Evidence from rural eastern India</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1568494620307304</t>
+  </si>
+  <si>
+    <t>Assessing countries’ performances against COVID-19 via WSIDEA and machine learning algorithms</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/full/10.1111/coin.12251</t>
+  </si>
+  <si>
+    <t>Efficiency analysis for stochastic dynamic facility layout problem using meta-heuristic, data envelopment analysis and machine learning</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0925527324000604#sec3</t>
+  </si>
+  <si>
+    <t>Using inverse DEA and machine learning algorithms to evaluate and predict suppliers’ performance in the apple supply chain</t>
   </si>
 </sst>
 </file>
@@ -80,12 +122,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -101,9 +149,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -439,121 +491,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0D959A-C41A-46F6-ABEE-5AEE7C58E141}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="131.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="131.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="76" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{3E674908-8178-43C6-A43C-F385A5FF4E01}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{317ED027-19F3-43DC-B422-04A4E0D4CB8E}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{3E674908-8178-43C6-A43C-F385A5FF4E01}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{317ED027-19F3-43DC-B422-04A4E0D4CB8E}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{C39AC317-8AAA-4661-8EE4-CED3CEDA6695}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{BDC42368-8DD7-47D9-AC03-A753281F566A}"/>
+    <hyperlink ref="D6" r:id="rId5" location="fig2" xr:uid="{3F2DA44A-EDDF-4BEB-972F-83F49E8903B8}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{E91BFFE8-7148-4589-BC77-8DEA429BD2B2}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{644864C4-17FF-4B71-8EC4-BB11A73BF331}"/>
+    <hyperlink ref="D9" r:id="rId8" location="sec3" xr:uid="{7B0CCE27-B4B4-466E-92A1-3AD454E82453}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>